<commit_message>
feat: correcciones y fin de la practica
</commit_message>
<xml_diff>
--- a/Practica1/Documentacion/StarDiagram.xlsx
+++ b/Practica1/Documentacion/StarDiagram.xlsx
@@ -203,10 +203,10 @@
     <t>booking_datetime</t>
   </si>
   <si>
-    <t>id_tiempo</t>
-  </si>
-  <si>
     <t>asiento</t>
+  </si>
+  <si>
+    <t>Fecha</t>
   </si>
 </sst>
 </file>
@@ -906,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" topLeftCell="K5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1049,7 +1049,7 @@
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.3">
       <c r="M11" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>55</v>
@@ -1271,7 +1271,7 @@
     </row>
     <row r="38" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M38" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q38" s="1" t="s">
         <v>29</v>

</xml_diff>